<commit_message>
Cleaned up folder deletion
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thimm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8660D2-F61E-4ACB-B0FA-4DCB08AD1608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCBCE8-5C73-410B-929D-91F42397C7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Investor</t>
   </si>
@@ -31,16 +31,10 @@
     <t>Committed Amount</t>
   </si>
   <si>
-    <t>Collected</t>
-  </si>
-  <si>
     <t>Delta Ventures</t>
   </si>
   <si>
     <t>SAAS Fund</t>
-  </si>
-  <si>
-    <t>₹0.00</t>
   </si>
   <si>
     <t>Waterfield Advisors</t>
@@ -424,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -435,10 +429,9 @@
     <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -449,112 +442,94 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>1800000</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="E2">
         <v>111111</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <v>1800000</v>
       </c>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>222222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3">
-        <v>222222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>2800000</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="E4">
         <v>333333</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>1200000</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="E5">
         <v>4444444</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
         <v>3000000</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6">
+        <v>14</v>
+      </c>
+      <c r="E6">
         <v>555555</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to strip out * from import headers
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FCBCE8-5C73-410B-929D-91F42397C7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA08DE7F-848A-4EE9-B5AC-BC76C35B4E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Investor</t>
   </si>
@@ -49,25 +49,7 @@
     <t>Arun Gupta</t>
   </si>
   <si>
-    <t>SPV</t>
-  </si>
-  <si>
-    <t>AAA</t>
-  </si>
-  <si>
-    <t>BBB</t>
-  </si>
-  <si>
-    <t>CCC</t>
-  </si>
-  <si>
-    <t>DDD</t>
-  </si>
-  <si>
-    <t>EEE</t>
-  </si>
-  <si>
-    <t>Phone</t>
+    <t>Folio No</t>
   </si>
 </sst>
 </file>
@@ -418,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -431,7 +413,7 @@
     <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,11 +426,8 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -458,14 +437,11 @@
       <c r="C2" s="1">
         <v>1800000</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>111111</v>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -475,14 +451,11 @@
       <c r="C3" s="1">
         <v>1800000</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>222222</v>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -492,14 +465,11 @@
       <c r="C4" s="1">
         <v>2800000</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>333333</v>
+      <c r="D4">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -509,14 +479,11 @@
       <c r="C5" s="1">
         <v>1200000</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>4444444</v>
+      <c r="D5">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -526,11 +493,8 @@
       <c r="C6" s="1">
         <v>3000000</v>
       </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>555555</v>
+      <c r="D6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 8 decimal places to capital commitment percentage
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93409B80-2EED-4F46-A0D8-410DCF8E8BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D662AD-9817-41D5-91D2-E8962F5BBFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Investor 4</t>
-  </si>
-  <si>
-    <t>Investor 5</t>
   </si>
 </sst>
 </file>
@@ -426,7 +423,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +505,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Added commitment date, to enable fx conversions on date
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168B76DB-D72F-4C72-8641-140A75F06F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82AD120-37A5-4303-B36C-AA37DC16E853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Series C1</t>
+  </si>
+  <si>
+    <t>Commitment Date</t>
   </si>
 </sst>
 </file>
@@ -138,10 +141,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J3" sqref="J3:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -472,9 +476,10 @@
     <col min="3" max="3" width="13.1875" customWidth="1"/>
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.875" customWidth="1"/>
+    <col min="10" max="10" width="9.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -502,8 +507,11 @@
       <c r="I1" t="s">
         <v>14</v>
       </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -528,8 +536,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="3">
+        <v>44946</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,8 +565,11 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
+      <c r="J3" s="3">
+        <v>44946</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -580,8 +594,11 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
+      <c r="J4" s="3">
+        <v>44946</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -606,8 +623,11 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
+      <c r="J5" s="3">
+        <v>44946</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -632,8 +652,11 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="3">
+        <v>44946</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -657,6 +680,9 @@
       </c>
       <c r="H7" t="s">
         <v>13</v>
+      </c>
+      <c r="J7" s="3">
+        <v>44946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commitment import now updates fields
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC239DF-E9CC-4C25-BF28-5CEBC6FFFB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59FC8D2-9F6E-44EB-8FFD-F8386EBF463D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>As Of</t>
+  </si>
+  <si>
+    <t>Onboarding Completed</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -153,12 +162,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I1" sqref="I1:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -489,10 +497,10 @@
     <col min="3" max="3" width="13.1875" customWidth="1"/>
     <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.875" customWidth="1"/>
-    <col min="10" max="10" width="9.9375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -518,25 +526,28 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -561,11 +572,14 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3">
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="3">
         <v>44946</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -590,11 +604,14 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3">
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="3">
         <v>44946</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -619,11 +636,14 @@
       <c r="H4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3">
+      <c r="I4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="3">
         <v>44946</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -648,11 +668,14 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3">
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="3">
         <v>44946</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -677,11 +700,14 @@
       <c r="H6" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3">
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="3">
         <v>44946</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -706,7 +732,10 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3">
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="3">
         <v>44946</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added normalization of key fields
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1256D1B9-736F-4F07-8295-0CC8ADFEFB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233E74CC-CAD4-4714-8CEB-1245057C9EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Commitment Date *</t>
+  </si>
+  <si>
+    <t>KYC Full Name</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -500,7 +503,7 @@
     <col min="11" max="11" width="16.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -546,8 +549,11 @@
       <c r="O1" t="s">
         <v>25</v>
       </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -579,7 +585,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -611,7 +617,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -643,7 +649,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,7 +681,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -707,7 +713,7 @@
         <v>44946</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixed bug in base notification for checking entity whastapp enabled
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00F33F5-ADFC-407B-A958-AD54856A032A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E25A36-FC8C-49E6-A5FB-9E64906CC99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>signatory2@gmail.com</t>
+  </si>
+  <si>
+    <t>Update Only</t>
   </si>
 </sst>
 </file>
@@ -515,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -532,7 +535,7 @@
     <col min="12" max="12" width="16.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -584,8 +587,11 @@
       <c r="Q1" t="s">
         <v>28</v>
       </c>
+      <c r="R1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -619,8 +625,11 @@
       <c r="L2" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="R2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -654,8 +663,11 @@
       <c r="L3" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="R3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -689,8 +701,11 @@
       <c r="L4" t="s">
         <v>35</v>
       </c>
+      <c r="R4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -724,8 +739,11 @@
       <c r="L5" t="s">
         <v>35</v>
       </c>
+      <c r="R5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -759,8 +777,11 @@
       <c r="L6" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -794,8 +815,11 @@
       <c r="L7" s="5" t="s">
         <v>34</v>
       </c>
+      <c r="R7" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -829,8 +853,11 @@
       <c r="L8" t="s">
         <v>35</v>
       </c>
+      <c r="R8" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -863,6 +890,9 @@
       </c>
       <c r="L9" t="s">
         <v>35</v>
+      </c>
+      <c r="R9" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom notifications per email (#211)
* Added email_method to custom_notifications

* Added email_method to custom_notifications

* Added custom notifications mail partial

* Refatored emails for custom notifications

* Added tests for custom notifications

* Added tests for custom notifications

* Changed Full Name to Investment Entity
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7639B4-DD4D-4234-B76E-1505271774E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CC0C29-DA32-4F36-8C97-64CBCF13AFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -597,9 +597,6 @@
     <t>Commitment Date *</t>
   </si>
   <si>
-    <t>KYC Full Name</t>
-  </si>
-  <si>
     <t>Committed   amount *</t>
   </si>
   <si>
@@ -622,6 +619,9 @@
   </si>
   <si>
     <t>Update Only</t>
+  </si>
+  <si>
+    <t>KYC Investing Entity</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K9"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1104,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>10</v>
@@ -1128,7 +1128,7 @@
         <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>20</v>
@@ -1143,10 +1143,10 @@
         <v>23</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S1" s="2"/>
     </row>
@@ -1182,7 +1182,7 @@
         <v>44946</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>26</v>
@@ -1220,7 +1220,7 @@
         <v>44946</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>26</v>
@@ -1258,7 +1258,7 @@
         <v>44946</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>26</v>
@@ -1296,7 +1296,7 @@
         <v>44946</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>26</v>
@@ -1334,7 +1334,7 @@
         <v>44946</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>26</v>
@@ -1372,7 +1372,7 @@
         <v>44946</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>26</v>
@@ -1380,7 +1380,7 @@
     </row>
     <row r="8" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1410,7 +1410,7 @@
         <v>44946</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>26</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="9" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -1448,7 +1448,7 @@
         <v>44946</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Import fund and folio amounts (#699)
* Added fund and folio amts for commitment imports

* Check for cc.document_folder in update_investor, to avoid no folder errors

* Added fund and folio amts for CRP imports

* Added fund currency cols for remittance imports

* Fixed fund unit tests

* Fix for no template when AE is generated
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments.xlsx
+++ b/public/sample_uploads/capital_commitments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CC0C29-DA32-4F36-8C97-64CBCF13AFE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DAF8D6-A2F7-400D-9BC0-557AF1821726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="98" windowWidth="23985" windowHeight="14264" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CapitalCommitment" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
+    <author>thimm</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{395C0591-C40D-4E08-80F9-182DADFD47FA}">
@@ -133,7 +134,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{AB03DE7C-A0EA-43AA-8FD3-BA0D7862E186}">
+    <comment ref="E1" authorId="1" shapeId="0" xr:uid="{1779CCF1-0B87-416F-A6E4-5F004FBF2AE9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>thimm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Leave blank if you want the system to convert based on FX rates entered by you in the system</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{AB03DE7C-A0EA-43AA-8FD3-BA0D7862E186}">
       <text>
         <r>
           <rPr>
@@ -157,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C4FD4EEE-657B-457B-A7A5-9CE8DAB505F0}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C4FD4EEE-657B-457B-A7A5-9CE8DAB505F0}">
       <text>
         <r>
           <rPr>
@@ -181,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B169B4CF-5DC1-4448-A8BE-33ED66179E89}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{B169B4CF-5DC1-4448-A8BE-33ED66179E89}">
       <text>
         <r>
           <rPr>
@@ -205,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{081F2FD3-7637-4B2F-B804-E2B64DADF4F5}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{081F2FD3-7637-4B2F-B804-E2B64DADF4F5}">
       <text>
         <r>
           <rPr>
@@ -229,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A935AABE-74E7-4099-BDC7-6CD3A74C100C}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A935AABE-74E7-4099-BDC7-6CD3A74C100C}">
       <text>
         <r>
           <rPr>
@@ -254,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{25DBCE79-B949-4E4D-BE57-70E789D34A3E}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{25DBCE79-B949-4E4D-BE57-70E789D34A3E}">
       <text>
         <r>
           <rPr>
@@ -278,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{2F96155C-E68E-4015-BACC-A3EACCCA4B52}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{2F96155C-E68E-4015-BACC-A3EACCCA4B52}">
       <text>
         <r>
           <rPr>
@@ -302,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{0D4B7892-34FB-4834-96B7-E6E216E05F80}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{0D4B7892-34FB-4834-96B7-E6E216E05F80}">
       <text>
         <r>
           <rPr>
@@ -326,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{05469727-1631-4829-8294-1949FFA88B0D}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{05469727-1631-4829-8294-1949FFA88B0D}">
       <text>
         <r>
           <rPr>
@@ -350,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{076F9775-548C-43DD-9EA7-66F1EDE2BED3}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{076F9775-548C-43DD-9EA7-66F1EDE2BED3}">
       <text>
         <r>
           <rPr>
@@ -374,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{F60F2AD9-95FA-4ACD-BE61-8A8031AA5F28}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{F60F2AD9-95FA-4ACD-BE61-8A8031AA5F28}">
       <text>
         <r>
           <rPr>
@@ -398,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A6B5CBA8-35C1-4DE2-BF9C-084E75CD31AE}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{A6B5CBA8-35C1-4DE2-BF9C-084E75CD31AE}">
       <text>
         <r>
           <rPr>
@@ -422,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{9E99BB9B-6DEA-446C-A59D-59F859533C17}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{9E99BB9B-6DEA-446C-A59D-59F859533C17}">
       <text>
         <r>
           <rPr>
@@ -446,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{2E2803F7-963F-46E7-9EBF-F7254C6F0D59}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{2E2803F7-963F-46E7-9EBF-F7254C6F0D59}">
       <text>
         <r>
           <rPr>
@@ -472,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{02D85A9C-43CD-45EC-BB93-23F1730E58EB}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{02D85A9C-43CD-45EC-BB93-23F1730E58EB}">
       <text>
         <r>
           <rPr>
@@ -511,7 +536,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -597,9 +622,6 @@
     <t>Commitment Date *</t>
   </si>
   <si>
-    <t>Committed   amount *</t>
-  </si>
-  <si>
     <t>unit type</t>
   </si>
   <si>
@@ -622,6 +644,12 @@
   </si>
   <si>
     <t>KYC Investing Entity</t>
+  </si>
+  <si>
+    <t>Committed Amount (Folio Currency) *</t>
+  </si>
+  <si>
+    <t>Committed Amount (Fund Currency)</t>
   </si>
 </sst>
 </file>
@@ -1064,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -1075,25 +1103,26 @@
     <col min="1" max="1" width="8.5625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.4375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.4375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.0625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.9375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.1875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.25" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.8125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="3"/>
+    <col min="4" max="4" width="32.3125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.4375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.0625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.9375" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.1875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.8125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1104,53 +1133,56 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="2"/>
-    </row>
-    <row r="2" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="S1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1163,32 +1195,33 @@
       <c r="D2" s="5">
         <v>1800000</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="10">
+      <c r="L2" s="10">
         <v>44946</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="M2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -1201,32 +1234,33 @@
       <c r="D3" s="5">
         <v>1800000</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="10">
+      <c r="L3" s="10">
         <v>44946</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="3" t="s">
+      <c r="M3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1239,32 +1273,33 @@
       <c r="D4" s="5">
         <v>2800000</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="10">
+      <c r="L4" s="10">
         <v>44946</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" s="3" t="s">
+      <c r="M4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -1277,32 +1312,33 @@
       <c r="D5" s="5">
         <v>1200000</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="10">
+      <c r="L5" s="10">
         <v>44946</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="3" t="s">
+      <c r="M5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1315,32 +1351,33 @@
       <c r="D6" s="5">
         <v>3000000</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="10">
+      <c r="L6" s="10">
         <v>44946</v>
       </c>
-      <c r="L6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" s="3" t="s">
+      <c r="M6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1353,34 +1390,35 @@
       <c r="D7" s="5">
         <v>1000000</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="10">
+      <c r="L7" s="10">
         <v>44946</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="3" t="s">
+      <c r="M7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -1391,34 +1429,35 @@
       <c r="D8" s="5">
         <v>3000000</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>11</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="10">
+      <c r="L8" s="10">
         <v>44946</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R8" s="3" t="s">
+      <c r="M8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -1429,32 +1468,33 @@
       <c r="D9" s="5">
         <v>3000000</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>12</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="10">
+      <c r="L9" s="10">
         <v>44946</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R9" s="3" t="s">
+      <c r="M9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A11"/>
       <c r="B11"/>
       <c r="D11"/>
@@ -1462,58 +1502,61 @@
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
-      <c r="J11"/>
+      <c r="I11"/>
       <c r="K11"/>
-      <c r="L11" s="7"/>
-      <c r="M11"/>
+      <c r="L11"/>
+      <c r="M11" s="7"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
       <c r="Q11"/>
-    </row>
-    <row r="12" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R11"/>
+    </row>
+    <row r="12" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A12"/>
       <c r="B12"/>
       <c r="D12" s="8"/>
-      <c r="E12"/>
+      <c r="E12" s="8"/>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12"/>
-      <c r="J12"/>
+      <c r="I12"/>
       <c r="K12"/>
-      <c r="L12" s="9"/>
-      <c r="M12"/>
+      <c r="L12"/>
+      <c r="M12" s="9"/>
       <c r="N12"/>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R12"/>
+    </row>
+    <row r="13" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A13"/>
       <c r="B13"/>
       <c r="D13" s="8"/>
-      <c r="E13"/>
+      <c r="E13" s="8"/>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13"/>
-      <c r="J13"/>
+      <c r="I13"/>
       <c r="K13"/>
-      <c r="L13" s="9"/>
-      <c r="M13"/>
+      <c r="L13"/>
+      <c r="M13" s="9"/>
       <c r="N13"/>
       <c r="O13"/>
       <c r="P13"/>
       <c r="Q13"/>
-    </row>
-    <row r="14" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R13"/>
+    </row>
+    <row r="14" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A14"/>
       <c r="B14"/>
       <c r="D14" s="8"/>
-      <c r="E14"/>
+      <c r="E14" s="8"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
-      <c r="J14"/>
+      <c r="I14"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -1521,16 +1564,17 @@
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R14"/>
+    </row>
+    <row r="15" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15"/>
       <c r="B15"/>
       <c r="D15" s="8"/>
-      <c r="E15"/>
+      <c r="E15" s="8"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
-      <c r="J15"/>
+      <c r="I15"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -1538,50 +1582,53 @@
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:19" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R15"/>
+    </row>
+    <row r="16" spans="1:20" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A16"/>
       <c r="B16"/>
       <c r="D16" s="8"/>
-      <c r="E16"/>
+      <c r="E16" s="8"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="J16"/>
+      <c r="I16"/>
       <c r="K16"/>
-      <c r="L16" s="9"/>
-      <c r="M16"/>
+      <c r="L16"/>
+      <c r="M16" s="9"/>
       <c r="N16"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
-    </row>
-    <row r="17" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R16"/>
+    </row>
+    <row r="17" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17"/>
       <c r="B17"/>
       <c r="D17" s="8"/>
-      <c r="E17"/>
+      <c r="E17" s="8"/>
       <c r="F17"/>
       <c r="G17"/>
       <c r="H17"/>
-      <c r="J17"/>
+      <c r="I17"/>
       <c r="K17"/>
-      <c r="L17" s="9"/>
-      <c r="M17"/>
+      <c r="L17"/>
+      <c r="M17" s="9"/>
       <c r="N17"/>
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
-    </row>
-    <row r="18" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R17"/>
+    </row>
+    <row r="18" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A18"/>
       <c r="B18"/>
       <c r="D18" s="8"/>
-      <c r="E18"/>
+      <c r="E18" s="8"/>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
-      <c r="J18"/>
+      <c r="I18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
@@ -1589,16 +1636,17 @@
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
-    </row>
-    <row r="19" spans="1:17" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="R18"/>
+    </row>
+    <row r="19" spans="1:18" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A19"/>
       <c r="B19"/>
       <c r="D19" s="8"/>
-      <c r="E19"/>
+      <c r="E19" s="8"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
-      <c r="J19"/>
+      <c r="I19"/>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19"/>
@@ -1606,24 +1654,25 @@
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
+      <c r="R19"/>
     </row>
   </sheetData>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{3242A391-47FF-4100-94F3-415E7E3E3E03}">
       <formula1>"Pool,CoInvest"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{21AA2D3E-6E60-4513-9535-8648FB8F7297}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{21AA2D3E-6E60-4513-9535-8648FB8F7297}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576" xr:uid="{24EBE599-D9A1-4410-B539-6461036AF991}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S1048576" xr:uid="{24EBE599-D9A1-4410-B539-6461036AF991}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{C20A9336-8299-41A8-97D5-E8960DDB86C9}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{311D3617-BDBE-4F9A-82A2-C604AF9C1482}"/>
-    <hyperlink ref="L6" r:id="rId3" xr:uid="{19F7B479-C653-4D40-B079-4EF7A04E9808}"/>
-    <hyperlink ref="L7" r:id="rId4" xr:uid="{66D3C224-6723-4429-9940-B3A4BAE8A52A}"/>
+    <hyperlink ref="M2" r:id="rId1" xr:uid="{C20A9336-8299-41A8-97D5-E8960DDB86C9}"/>
+    <hyperlink ref="M3" r:id="rId2" xr:uid="{311D3617-BDBE-4F9A-82A2-C604AF9C1482}"/>
+    <hyperlink ref="M6" r:id="rId3" xr:uid="{19F7B479-C653-4D40-B079-4EF7A04E9808}"/>
+    <hyperlink ref="M7" r:id="rId4" xr:uid="{66D3C224-6723-4429-9940-B3A4BAE8A52A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>

</xml_diff>